<commit_message>
To make nomenclature more consistent, changed some argument names and changed "Larvae" to "Larva"
</commit_message>
<xml_diff>
--- a/data-raw/undersampled.xlsx
+++ b/data-raw/undersampled.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\ZoopSynth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58564347-6B4D-406D-A158-4B3F7F8D437F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28755" windowHeight="12105"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +51,6 @@
     <t>Copepoda</t>
   </si>
   <si>
-    <t>Larvae</t>
-  </si>
-  <si>
     <t>Eurytemora affinis</t>
   </si>
   <si>
@@ -111,12 +109,15 @@
   </si>
   <si>
     <t>Oithona similis</t>
+  </si>
+  <si>
+    <t>Larva</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,11 +447,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +490,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -497,10 +498,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -508,10 +509,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -519,7 +520,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -530,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -541,10 +542,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -552,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -563,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -574,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -585,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -596,10 +597,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -607,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -618,10 +619,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -629,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
@@ -640,10 +641,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -662,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -673,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -684,10 +685,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -695,7 +696,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -706,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Updated crosswalk with DOP data and adjsuted zoopdownloader to download DOP data.
</commit_message>
<xml_diff>
--- a/data-raw/undersampled.xlsx
+++ b/data-raw/undersampled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/ZoopSynth/zooper/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58564347-6B4D-406D-A158-4B3F7F8D437F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{58564347-6B4D-406D-A158-4B3F7F8D437F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E776DFF4-7781-4583-B1BF-37C16FB0330F}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="29">
   <si>
     <t>SizeClass</t>
   </si>
@@ -448,19 +448,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -482,7 +482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -493,7 +493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -504,7 +504,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -526,7 +526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -537,7 +537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -548,7 +548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -559,7 +559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -570,7 +570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -581,7 +581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -592,7 +592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -603,7 +603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -614,7 +614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -625,7 +625,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
@@ -636,7 +636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -647,7 +647,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
@@ -658,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -669,7 +669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -680,7 +680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -691,7 +691,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -702,7 +702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -710,6 +710,61 @@
         <v>27</v>
       </c>
       <c r="C23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed the rounding on the zoopsynther test, added source dataset tests, minor tweaks to zoopdownloader
</commit_message>
<xml_diff>
--- a/data-raw/undersampled.xlsx
+++ b/data-raw/undersampled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/ZoopSynth/zooper/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{58564347-6B4D-406D-A158-4B3F7F8D437F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E776DFF4-7781-4583-B1BF-37C16FB0330F}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{58564347-6B4D-406D-A158-4B3F7F8D437F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3CB3EA0-15B5-47A4-B23E-E137C6F5D62F}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>